<commit_message>
Inclusão de Materiais de Consumo
Permitido agora incluir vários materiais de consumo - Valores e Tipos
serão trazidos do cadastro.
</commit_message>
<xml_diff>
--- a/web/uploads/imports/materalconsumo.xlsx
+++ b/web/uploads/imports/materalconsumo.xlsx
@@ -560,7 +560,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,15 +596,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -878,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,6 +900,7 @@
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -899,7 +913,7 @@
       <c r="C1" t="s">
         <v>167</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>168</v>
       </c>
       <c r="E1" t="s">
@@ -916,8 +930,8 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
-        <v>4.7576486842105261</v>
+      <c r="D2" s="2">
+        <v>4.76</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -933,7 +947,7 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>17.5</v>
       </c>
       <c r="E3">
@@ -951,7 +965,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="1">
-        <v>50.449999999999996</v>
+        <v>50.45</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -968,7 +982,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="1">
-        <v>4.002319858156028</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1002,7 +1016,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="1">
-        <v>14.352175000000001</v>
+        <v>14.35</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1104,7 +1118,7 @@
         <v>16</v>
       </c>
       <c r="D13" s="1">
-        <v>30.277575757575757</v>
+        <v>30.3</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1189,7 +1203,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="1">
-        <v>19.721699999999998</v>
+        <v>19.7</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1257,7 +1271,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="1">
-        <v>14.965116666666667</v>
+        <v>15</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1291,7 +1305,7 @@
         <v>29</v>
       </c>
       <c r="D24" s="1">
-        <v>3.614698717948718</v>
+        <v>3.6</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1427,7 +1441,7 @@
         <v>4</v>
       </c>
       <c r="D32" s="1">
-        <v>14.99</v>
+        <v>15</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1478,7 +1492,7 @@
         <v>4</v>
       </c>
       <c r="D35" s="1">
-        <v>9.374769620253165</v>
+        <v>9.4</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1495,7 +1509,7 @@
         <v>41</v>
       </c>
       <c r="D36" s="1">
-        <v>8.4376499999999997</v>
+        <v>8.5</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1665,7 +1679,7 @@
         <v>4</v>
       </c>
       <c r="D46" s="1">
-        <v>6.261825</v>
+        <v>6.3</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1682,7 +1696,7 @@
         <v>4</v>
       </c>
       <c r="D47" s="1">
-        <v>7.7764220000000002</v>
+        <v>7.8</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1801,7 +1815,7 @@
         <v>4</v>
       </c>
       <c r="D54" s="1">
-        <v>13.649425806451614</v>
+        <v>13.7</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -2039,7 +2053,7 @@
         <v>4</v>
       </c>
       <c r="D68" s="1">
-        <v>8.6077777777777769</v>
+        <v>8.6</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -2379,7 +2393,7 @@
         <v>4</v>
       </c>
       <c r="D88" s="1">
-        <v>22.815948905109487</v>
+        <v>22.8</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -2413,7 +2427,7 @@
         <v>4</v>
       </c>
       <c r="D90" s="1">
-        <v>42.589999999999996</v>
+        <v>43</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -2430,7 +2444,7 @@
         <v>4</v>
       </c>
       <c r="D91" s="1">
-        <v>19.920187755102042</v>
+        <v>20</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -2634,7 +2648,7 @@
         <v>4</v>
       </c>
       <c r="D103" s="1">
-        <v>35.993500000000004</v>
+        <v>36</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -2685,7 +2699,7 @@
         <v>88</v>
       </c>
       <c r="D106" s="1">
-        <v>25.256180000000001</v>
+        <v>25.25</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -2702,7 +2716,7 @@
         <v>88</v>
       </c>
       <c r="D107" s="1">
-        <v>10.9725</v>
+        <v>11</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -2736,7 +2750,7 @@
         <v>4</v>
       </c>
       <c r="D109" s="1">
-        <v>19.899999999999999</v>
+        <v>20</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -2787,7 +2801,7 @@
         <v>4</v>
       </c>
       <c r="D112" s="1">
-        <v>16.989999999999998</v>
+        <v>17</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -2872,7 +2886,7 @@
         <v>41</v>
       </c>
       <c r="D117" s="1">
-        <v>6.4032099999999996</v>
+        <v>6.4</v>
       </c>
       <c r="E117">
         <v>1</v>
@@ -3450,7 +3464,7 @@
         <v>4</v>
       </c>
       <c r="D151" s="1">
-        <v>5.4200000000000008</v>
+        <v>5.42</v>
       </c>
       <c r="E151">
         <v>1</v>
@@ -3467,7 +3481,7 @@
         <v>4</v>
       </c>
       <c r="D152" s="1">
-        <v>5.4200000000000008</v>
+        <v>5.42</v>
       </c>
       <c r="E152">
         <v>1</v>
@@ -3569,7 +3583,7 @@
         <v>4</v>
       </c>
       <c r="D158" s="1">
-        <v>4.99</v>
+        <v>5</v>
       </c>
       <c r="E158">
         <v>1</v>

</xml_diff>